<commit_message>
Sign Up page and cross compatibility issue unresolved
</commit_message>
<xml_diff>
--- a/WorkLog.xlsx
+++ b/WorkLog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F1C193-AED8-4C86-B24B-FE7F436F705C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8425046E-56DD-449A-8217-F0D5286C9E0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Work Done</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Creating Login</t>
   </si>
   <si>
-    <t>Creating Register</t>
-  </si>
-  <si>
     <t>2 pm - 3 pm</t>
   </si>
   <si>
@@ -134,6 +131,33 @@
   </si>
   <si>
     <t>9 pm - 10:30 pm</t>
+  </si>
+  <si>
+    <t>Knowledge training</t>
+  </si>
+  <si>
+    <t>Karan and Amandeep</t>
+  </si>
+  <si>
+    <t>Amandeep</t>
+  </si>
+  <si>
+    <t>11 AM - 12 pm</t>
+  </si>
+  <si>
+    <t>9 am - 10:45 am</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Creating SignUp</t>
+  </si>
+  <si>
+    <t>Cross Compatibilty issue</t>
+  </si>
+  <si>
+    <t>Review needed!</t>
   </si>
 </sst>
 </file>
@@ -166,12 +190,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -186,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -195,6 +225,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +460,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -477,7 +524,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -491,7 +538,7 @@
         <v>43874</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -505,7 +552,7 @@
         <v>43874</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>12</v>
@@ -513,13 +560,13 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4">
         <v>43874</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>12</v>
@@ -533,7 +580,7 @@
         <v>43874</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -547,10 +594,10 @@
         <v>43874</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>12</v>
@@ -558,118 +605,159 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4">
+        <v>43874</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4">
-        <v>43874</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4">
         <v>43874</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4">
         <v>43874</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4">
+        <v>43874</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="4">
-        <v>43874</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4">
         <v>43874</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="4">
+        <v>43874</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="4">
-        <v>43874</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4">
+        <v>43875</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="4">
+        <v>43875</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="11">
+        <v>43875</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>